<commit_message>
fixed run description table error
</commit_message>
<xml_diff>
--- a/runs/v23/SwabSeqv23.xlsx
+++ b/runs/v23/SwabSeqv23.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="_constants" sheetId="1" state="visible" r:id="rId2"/>
@@ -4567,7 +4567,7 @@
   </sheetPr>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -5169,7 +5169,7 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -7158,7 +7158,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.780612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -7919,8 +7919,8 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>